<commit_message>
merging looking good for all but ncaab
</commit_message>
<xml_diff>
--- a/Data/Odds/NCAAF/ncaa football 2021-22.xlsx
+++ b/Data/Odds/NCAAF/ncaa football 2021-22.xlsx
@@ -3538,10 +3538,8 @@
       <c r="I68" t="n">
         <v>28</v>
       </c>
-      <c r="J68" t="inlineStr">
-        <is>
-          <t>7.5ev</t>
-        </is>
+      <c r="J68" t="n">
+        <v>7.5</v>
       </c>
       <c r="K68" t="n">
         <v>6.5</v>

</xml_diff>

<commit_message>
all league datasets merged
</commit_message>
<xml_diff>
--- a/Data/Odds/NCAAF/ncaa football 2021-22.xlsx
+++ b/Data/Odds/NCAAF/ncaa football 2021-22.xlsx
@@ -40828,10 +40828,8 @@
       <c r="I888" t="n">
         <v>55</v>
       </c>
-      <c r="J888" t="inlineStr">
-        <is>
-          <t>1..5</t>
-        </is>
+      <c r="J888" t="n">
+        <v>1.5</v>
       </c>
       <c r="K888" t="n">
         <v>1</v>

</xml_diff>